<commit_message>
Remove unused files, refactor create_conciliation for improved discrepancy handling
</commit_message>
<xml_diff>
--- a/format.xlsx
+++ b/format.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="29029"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="29127"/>
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\jezrr\Dev\YuGPT\back\YuGPT-Server\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/76f1a75cf433d042/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{50A64EC1-1621-4EC1-99E7-6A61C96270CB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="23" documentId="8_{1658749F-1375-4E6A-A401-979035052B8B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{DE03ED7A-FAD4-4D69-9E9C-5C2E394A84F5}"/>
   <bookViews>
-    <workbookView xWindow="-98" yWindow="-98" windowWidth="19396" windowHeight="11475" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="NOVIEMBRE" sheetId="1" r:id="rId1"/>
@@ -27,8 +27,6 @@
         <xcalcf:feature name="microsoft.com:FV"/>
         <xcalcf:feature name="microsoft.com:CNMTM"/>
         <xcalcf:feature name="microsoft.com:LET_WF"/>
-        <xcalcf:feature name="microsoft.com:LAMBDA_WF"/>
-        <xcalcf:feature name="microsoft.com:ARRAYTEXT_WF"/>
       </xcalcf:calcFeatures>
     </ext>
     <ext xmlns:loext="http://schemas.libreoffice.org/" uri="{7626C862-2A13-11E5-B345-FEFF819CDC9F}">
@@ -87,15 +85,13 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <numFmts count="6">
+  <numFmts count="4">
     <numFmt numFmtId="164" formatCode="_-* #,##0.00_-;\-* #,##0.00_-;_-* \-??_-;_-@_-"/>
-    <numFmt numFmtId="165" formatCode="dd\-mmm\-yy"/>
-    <numFmt numFmtId="166" formatCode="_(* #,##0.00_);_(* \(#,##0.00\);_(* \-??_);_(@_)"/>
-    <numFmt numFmtId="167" formatCode="_-\$* #,##0.00_-;&quot;-$&quot;* #,##0.00_-;_-\$* \-??_-;_-@_-"/>
-    <numFmt numFmtId="168" formatCode="dd/mm/yyyy"/>
-    <numFmt numFmtId="169" formatCode="_-* #,##0.0000_-;\-* #,##0.0000_-;_-* \-??_-;_-@_-"/>
+    <numFmt numFmtId="165" formatCode="_(* #,##0.00_);_(* \(#,##0.00\);_(* \-??_);_(@_)"/>
+    <numFmt numFmtId="166" formatCode="_-\$* #,##0.00_-;&quot;-$&quot;* #,##0.00_-;_-\$* \-??_-;_-@_-"/>
+    <numFmt numFmtId="167" formatCode="_-* #,##0.0000_-;\-* #,##0.0000_-;_-* \-??_-;_-@_-"/>
   </numFmts>
-  <fonts count="11" x14ac:knownFonts="1">
+  <fonts count="11">
     <font>
       <sz val="11"/>
       <color rgb="FF000000"/>
@@ -222,7 +218,7 @@
   <cellStyleXfs count="5">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="164" fontId="10" fillId="0" borderId="0" applyBorder="0" applyProtection="0"/>
-    <xf numFmtId="167" fontId="10" fillId="0" borderId="0" applyBorder="0" applyProtection="0"/>
+    <xf numFmtId="166" fontId="10" fillId="0" borderId="0" applyBorder="0" applyProtection="0"/>
     <xf numFmtId="164" fontId="10" fillId="0" borderId="0" applyBorder="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="10" fillId="0" borderId="0"/>
   </cellStyleXfs>
@@ -248,7 +244,7 @@
     </xf>
     <xf numFmtId="164" fontId="1" fillId="0" borderId="0" xfId="3" applyFont="1" applyBorder="1" applyProtection="1"/>
     <xf numFmtId="49" fontId="1" fillId="0" borderId="0" xfId="4" applyNumberFormat="1" applyFont="1"/>
-    <xf numFmtId="165" fontId="7" fillId="0" borderId="0" xfId="4" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+    <xf numFmtId="15" fontId="7" fillId="0" borderId="0" xfId="4" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment vertical="top"/>
     </xf>
     <xf numFmtId="164" fontId="4" fillId="0" borderId="1" xfId="3" applyFont="1" applyBorder="1" applyProtection="1"/>
@@ -263,8 +259,8 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="4" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="166" fontId="1" fillId="0" borderId="0" xfId="4" applyNumberFormat="1" applyFont="1"/>
-    <xf numFmtId="166" fontId="1" fillId="0" borderId="1" xfId="4" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="165" fontId="1" fillId="0" borderId="0" xfId="4" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="165" fontId="1" fillId="0" borderId="1" xfId="4" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
     <xf numFmtId="164" fontId="1" fillId="0" borderId="1" xfId="1" applyFont="1" applyBorder="1" applyProtection="1"/>
     <xf numFmtId="164" fontId="1" fillId="0" borderId="0" xfId="1" applyFont="1" applyBorder="1" applyProtection="1"/>
     <xf numFmtId="164" fontId="8" fillId="0" borderId="0" xfId="1" applyFont="1" applyBorder="1" applyProtection="1"/>
@@ -272,20 +268,20 @@
     <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="49" fontId="4" fillId="0" borderId="0" xfId="3" applyNumberFormat="1" applyFont="1" applyBorder="1" applyProtection="1"/>
     <xf numFmtId="164" fontId="1" fillId="0" borderId="1" xfId="3" applyFont="1" applyBorder="1" applyProtection="1"/>
-    <xf numFmtId="166" fontId="10" fillId="0" borderId="0" xfId="4" applyNumberFormat="1"/>
+    <xf numFmtId="165" fontId="10" fillId="0" borderId="0" xfId="4" applyNumberFormat="1"/>
     <xf numFmtId="164" fontId="1" fillId="0" borderId="2" xfId="1" applyFont="1" applyBorder="1" applyProtection="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="4" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="167" fontId="8" fillId="0" borderId="0" xfId="2" applyFont="1" applyBorder="1" applyProtection="1"/>
-    <xf numFmtId="168" fontId="1" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyProtection="1"/>
-    <xf numFmtId="169" fontId="1" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyProtection="1"/>
+    <xf numFmtId="166" fontId="8" fillId="0" borderId="0" xfId="2" applyFont="1" applyBorder="1" applyProtection="1"/>
+    <xf numFmtId="14" fontId="1" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyProtection="1"/>
+    <xf numFmtId="167" fontId="1" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyProtection="1"/>
     <xf numFmtId="164" fontId="4" fillId="0" borderId="0" xfId="3" applyFont="1" applyBorder="1" applyProtection="1"/>
-    <xf numFmtId="166" fontId="4" fillId="0" borderId="3" xfId="4" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="166" fontId="4" fillId="0" borderId="0" xfId="4" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="165" fontId="4" fillId="0" borderId="3" xfId="4" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="165" fontId="4" fillId="0" borderId="0" xfId="4" applyNumberFormat="1" applyFont="1"/>
   </cellXfs>
   <cellStyles count="5">
-    <cellStyle name="Comma" xfId="1" builtinId="3"/>
     <cellStyle name="Comma 2" xfId="3" xr:uid="{00000000-0005-0000-0000-000006000000}"/>
-    <cellStyle name="Currency" xfId="2" builtinId="4"/>
+    <cellStyle name="Millares" xfId="1" builtinId="3"/>
+    <cellStyle name="Moneda" xfId="2" builtinId="4"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
     <cellStyle name="Normal 2" xfId="4" xr:uid="{00000000-0005-0000-0000-000007000000}"/>
   </cellStyles>
@@ -371,7 +367,7 @@
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Tema de Office">
   <a:themeElements>
     <a:clrScheme name="Office">
       <a:dk1>
@@ -690,21 +686,21 @@
   <sheetPr>
     <tabColor rgb="FF7030A0"/>
   </sheetPr>
-  <dimension ref="A1:N52"/>
+  <dimension ref="A1:O52"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="78" zoomScaleNormal="160" workbookViewId="0">
-      <selection activeCell="H10" sqref="H10"/>
+    <sheetView tabSelected="1" zoomScale="53" zoomScaleNormal="160" workbookViewId="0">
+      <selection activeCell="I28" sqref="I28"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.33203125" defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="11.296875" defaultRowHeight="13.8"/>
   <cols>
-    <col min="4" max="4" width="7.53125" customWidth="1"/>
-    <col min="5" max="5" width="12.33203125" customWidth="1"/>
+    <col min="4" max="4" width="7.5" customWidth="1"/>
+    <col min="5" max="5" width="12.296875" customWidth="1"/>
     <col min="8" max="8" width="13.796875" customWidth="1"/>
-    <col min="9" max="9" width="12.33203125" customWidth="1"/>
+    <col min="9" max="9" width="12.296875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:14" x14ac:dyDescent="0.45">
+    <row r="1" spans="1:15">
       <c r="A1" s="1"/>
       <c r="B1" s="2" t="s">
         <v>0</v>
@@ -720,7 +716,7 @@
       <c r="K1" s="1"/>
       <c r="L1" s="1"/>
     </row>
-    <row r="2" spans="1:14" x14ac:dyDescent="0.45">
+    <row r="2" spans="1:15">
       <c r="A2" s="1"/>
       <c r="B2" s="2" t="s">
         <v>1</v>
@@ -736,7 +732,7 @@
       <c r="K2" s="1"/>
       <c r="L2" s="1"/>
     </row>
-    <row r="3" spans="1:14" x14ac:dyDescent="0.45">
+    <row r="3" spans="1:15">
       <c r="A3" s="1"/>
       <c r="B3" s="2" t="s">
         <v>2</v>
@@ -752,10 +748,10 @@
       <c r="K3" s="1"/>
       <c r="L3" s="1"/>
     </row>
-    <row r="4" spans="1:14" x14ac:dyDescent="0.45">
+    <row r="4" spans="1:15">
       <c r="B4" s="2"/>
     </row>
-    <row r="5" spans="1:14" x14ac:dyDescent="0.45">
+    <row r="5" spans="1:15">
       <c r="A5" s="1"/>
       <c r="B5" s="1"/>
       <c r="C5" s="1"/>
@@ -769,7 +765,7 @@
       <c r="K5" s="9"/>
       <c r="L5" s="9"/>
     </row>
-    <row r="6" spans="1:14" x14ac:dyDescent="0.45">
+    <row r="6" spans="1:15">
       <c r="A6" s="1"/>
       <c r="B6" s="10" t="s">
         <v>3</v>
@@ -785,7 +781,7 @@
       <c r="K6" s="9"/>
       <c r="L6" s="9"/>
     </row>
-    <row r="7" spans="1:14" x14ac:dyDescent="0.45">
+    <row r="7" spans="1:15">
       <c r="A7" s="1"/>
       <c r="B7" s="1"/>
       <c r="C7" s="14"/>
@@ -799,7 +795,7 @@
       <c r="K7" s="9"/>
       <c r="L7" s="9"/>
     </row>
-    <row r="8" spans="1:14" x14ac:dyDescent="0.45">
+    <row r="8" spans="1:15">
       <c r="A8" s="1"/>
       <c r="B8" s="1"/>
       <c r="C8" s="1"/>
@@ -813,7 +809,7 @@
       <c r="K8" s="9"/>
       <c r="L8" s="9"/>
     </row>
-    <row r="9" spans="1:14" x14ac:dyDescent="0.45">
+    <row r="9" spans="1:15">
       <c r="A9" s="1"/>
       <c r="B9" s="15" t="s">
         <v>4</v>
@@ -824,7 +820,7 @@
       <c r="F9" s="17"/>
       <c r="G9" s="18"/>
       <c r="H9" s="19">
-        <f>SUM(A10:G15)</f>
+        <f>SUM(A10:G15, I10:O15)</f>
         <v>0</v>
       </c>
       <c r="I9" s="1"/>
@@ -832,7 +828,7 @@
       <c r="K9" s="9"/>
       <c r="L9" s="9"/>
     </row>
-    <row r="10" spans="1:14" x14ac:dyDescent="0.45">
+    <row r="10" spans="1:15">
       <c r="A10" s="20"/>
       <c r="B10" s="21"/>
       <c r="C10" s="20"/>
@@ -841,14 +837,15 @@
       <c r="F10" s="21"/>
       <c r="G10" s="20"/>
       <c r="H10" s="23"/>
-      <c r="I10" s="1"/>
+      <c r="I10" s="20"/>
       <c r="J10" s="1"/>
-      <c r="K10" s="9"/>
+      <c r="K10" s="20"/>
       <c r="L10" s="5"/>
-      <c r="M10" s="1"/>
+      <c r="M10" s="20"/>
       <c r="N10" s="1"/>
-    </row>
-    <row r="11" spans="1:14" x14ac:dyDescent="0.45">
+      <c r="O10" s="20"/>
+    </row>
+    <row r="11" spans="1:15">
       <c r="A11" s="20"/>
       <c r="B11" s="21"/>
       <c r="C11" s="20"/>
@@ -856,14 +853,15 @@
       <c r="E11" s="20"/>
       <c r="F11" s="21"/>
       <c r="G11" s="20"/>
-      <c r="I11" s="1"/>
+      <c r="I11" s="20"/>
       <c r="J11" s="1"/>
-      <c r="K11" s="9"/>
+      <c r="K11" s="20"/>
       <c r="L11" s="2"/>
-      <c r="M11" s="1"/>
+      <c r="M11" s="20"/>
       <c r="N11" s="2"/>
-    </row>
-    <row r="12" spans="1:14" x14ac:dyDescent="0.45">
+      <c r="O11" s="20"/>
+    </row>
+    <row r="12" spans="1:15">
       <c r="A12" s="20"/>
       <c r="B12" s="21"/>
       <c r="C12" s="20"/>
@@ -872,12 +870,14 @@
       <c r="F12" s="21"/>
       <c r="G12" s="20"/>
       <c r="H12" s="1"/>
-      <c r="I12" s="1"/>
+      <c r="I12" s="20"/>
       <c r="J12" s="1"/>
-      <c r="K12" s="9"/>
+      <c r="K12" s="20"/>
       <c r="L12" s="9"/>
-    </row>
-    <row r="13" spans="1:14" x14ac:dyDescent="0.45">
+      <c r="M12" s="20"/>
+      <c r="O12" s="20"/>
+    </row>
+    <row r="13" spans="1:15">
       <c r="A13" s="20"/>
       <c r="B13" s="21"/>
       <c r="C13" s="20"/>
@@ -886,12 +886,14 @@
       <c r="F13" s="21"/>
       <c r="G13" s="20"/>
       <c r="H13" s="1"/>
-      <c r="I13" s="1"/>
+      <c r="I13" s="20"/>
       <c r="J13" s="1"/>
-      <c r="K13" s="9"/>
+      <c r="K13" s="20"/>
       <c r="L13" s="9"/>
-    </row>
-    <row r="14" spans="1:14" x14ac:dyDescent="0.45">
+      <c r="M13" s="20"/>
+      <c r="O13" s="20"/>
+    </row>
+    <row r="14" spans="1:15">
       <c r="A14" s="20"/>
       <c r="B14" s="21"/>
       <c r="C14" s="20"/>
@@ -900,12 +902,14 @@
       <c r="F14" s="21"/>
       <c r="G14" s="20"/>
       <c r="H14" s="1"/>
-      <c r="I14" s="1"/>
+      <c r="I14" s="20"/>
       <c r="J14" s="1"/>
-      <c r="K14" s="9"/>
+      <c r="K14" s="20"/>
       <c r="L14" s="9"/>
-    </row>
-    <row r="15" spans="1:14" x14ac:dyDescent="0.45">
+      <c r="M14" s="20"/>
+      <c r="O14" s="20"/>
+    </row>
+    <row r="15" spans="1:15">
       <c r="A15" s="20"/>
       <c r="B15" s="21"/>
       <c r="C15" s="20"/>
@@ -914,12 +918,14 @@
       <c r="F15" s="21"/>
       <c r="G15" s="20"/>
       <c r="H15" s="1"/>
-      <c r="I15" s="1"/>
+      <c r="I15" s="20"/>
       <c r="J15" s="1"/>
-      <c r="K15" s="9"/>
+      <c r="K15" s="20"/>
       <c r="L15" s="9"/>
-    </row>
-    <row r="16" spans="1:14" x14ac:dyDescent="0.45">
+      <c r="M15" s="20"/>
+      <c r="O15" s="20"/>
+    </row>
+    <row r="16" spans="1:15">
       <c r="A16" s="21"/>
       <c r="B16" s="24"/>
       <c r="C16" s="21"/>
@@ -933,7 +939,7 @@
       <c r="K16" s="9"/>
       <c r="L16" s="9"/>
     </row>
-    <row r="17" spans="1:12" x14ac:dyDescent="0.45">
+    <row r="17" spans="1:15">
       <c r="A17" s="21"/>
       <c r="B17" s="25" t="s">
         <v>5</v>
@@ -944,7 +950,7 @@
       <c r="F17" s="2"/>
       <c r="G17" s="9"/>
       <c r="H17" s="26">
-        <f>SUM(A18:G23)</f>
+        <f>SUM(A18:G23, I18:O23)</f>
         <v>0</v>
       </c>
       <c r="I17" s="1"/>
@@ -952,7 +958,7 @@
       <c r="K17" s="9"/>
       <c r="L17" s="9"/>
     </row>
-    <row r="18" spans="1:12" x14ac:dyDescent="0.45">
+    <row r="18" spans="1:15">
       <c r="A18" s="20"/>
       <c r="B18" s="21"/>
       <c r="C18" s="20"/>
@@ -961,12 +967,15 @@
       <c r="F18" s="21"/>
       <c r="G18" s="20"/>
       <c r="H18" s="1"/>
-      <c r="I18" s="1"/>
+      <c r="I18" s="20"/>
       <c r="J18" s="1"/>
-      <c r="K18" s="9"/>
-      <c r="L18" s="9"/>
-    </row>
-    <row r="19" spans="1:12" x14ac:dyDescent="0.45">
+      <c r="K18" s="20"/>
+      <c r="L18" s="5"/>
+      <c r="M18" s="20"/>
+      <c r="N18" s="1"/>
+      <c r="O18" s="20"/>
+    </row>
+    <row r="19" spans="1:15">
       <c r="A19" s="20"/>
       <c r="B19" s="21"/>
       <c r="C19" s="20"/>
@@ -975,12 +984,15 @@
       <c r="F19" s="21"/>
       <c r="G19" s="20"/>
       <c r="H19" s="1"/>
-      <c r="I19" s="1"/>
+      <c r="I19" s="20"/>
       <c r="J19" s="1"/>
-      <c r="K19" s="9"/>
-      <c r="L19" s="9"/>
-    </row>
-    <row r="20" spans="1:12" x14ac:dyDescent="0.45">
+      <c r="K19" s="20"/>
+      <c r="L19" s="2"/>
+      <c r="M19" s="20"/>
+      <c r="N19" s="2"/>
+      <c r="O19" s="20"/>
+    </row>
+    <row r="20" spans="1:15">
       <c r="A20" s="20"/>
       <c r="B20" s="21"/>
       <c r="C20" s="20"/>
@@ -989,12 +1001,14 @@
       <c r="F20" s="21"/>
       <c r="G20" s="20"/>
       <c r="H20" s="1"/>
-      <c r="I20" s="1"/>
+      <c r="I20" s="20"/>
       <c r="J20" s="1"/>
-      <c r="K20" s="9"/>
+      <c r="K20" s="20"/>
       <c r="L20" s="9"/>
-    </row>
-    <row r="21" spans="1:12" x14ac:dyDescent="0.45">
+      <c r="M20" s="20"/>
+      <c r="O20" s="20"/>
+    </row>
+    <row r="21" spans="1:15">
       <c r="A21" s="20"/>
       <c r="B21" s="21"/>
       <c r="C21" s="20"/>
@@ -1003,12 +1017,14 @@
       <c r="F21" s="21"/>
       <c r="G21" s="20"/>
       <c r="H21" s="1"/>
-      <c r="I21" s="1"/>
+      <c r="I21" s="20"/>
       <c r="J21" s="1"/>
-      <c r="K21" s="9"/>
+      <c r="K21" s="20"/>
       <c r="L21" s="9"/>
-    </row>
-    <row r="22" spans="1:12" x14ac:dyDescent="0.45">
+      <c r="M21" s="20"/>
+      <c r="O21" s="20"/>
+    </row>
+    <row r="22" spans="1:15">
       <c r="A22" s="20"/>
       <c r="B22" s="21"/>
       <c r="C22" s="20"/>
@@ -1016,12 +1032,14 @@
       <c r="E22" s="20"/>
       <c r="F22" s="21"/>
       <c r="G22" s="20"/>
-      <c r="I22" s="1"/>
+      <c r="I22" s="20"/>
       <c r="J22" s="1"/>
-      <c r="K22" s="9"/>
+      <c r="K22" s="20"/>
       <c r="L22" s="9"/>
-    </row>
-    <row r="23" spans="1:12" x14ac:dyDescent="0.45">
+      <c r="M22" s="20"/>
+      <c r="O22" s="20"/>
+    </row>
+    <row r="23" spans="1:15">
       <c r="A23" s="20"/>
       <c r="B23" s="21"/>
       <c r="C23" s="20"/>
@@ -1030,12 +1048,14 @@
       <c r="F23" s="21"/>
       <c r="G23" s="20"/>
       <c r="H23" s="27"/>
-      <c r="I23" s="1"/>
-      <c r="J23" s="13"/>
-      <c r="K23" s="9"/>
+      <c r="I23" s="20"/>
+      <c r="J23" s="1"/>
+      <c r="K23" s="20"/>
       <c r="L23" s="9"/>
-    </row>
-    <row r="24" spans="1:12" x14ac:dyDescent="0.45">
+      <c r="M23" s="20"/>
+      <c r="O23" s="20"/>
+    </row>
+    <row r="24" spans="1:15">
       <c r="A24" s="21"/>
       <c r="B24" s="21"/>
       <c r="C24" s="21"/>
@@ -1048,7 +1068,7 @@
       <c r="K24" s="9"/>
       <c r="L24" s="9"/>
     </row>
-    <row r="25" spans="1:12" x14ac:dyDescent="0.45">
+    <row r="25" spans="1:15">
       <c r="E25" s="2" t="s">
         <v>12</v>
       </c>
@@ -1062,7 +1082,7 @@
       <c r="K25" s="9"/>
       <c r="L25" s="9"/>
     </row>
-    <row r="26" spans="1:12" x14ac:dyDescent="0.45">
+    <row r="26" spans="1:15">
       <c r="A26" s="28"/>
       <c r="B26" s="28"/>
       <c r="C26" s="28"/>
@@ -1076,7 +1096,7 @@
       <c r="K26" s="9"/>
       <c r="L26" s="9"/>
     </row>
-    <row r="27" spans="1:12" x14ac:dyDescent="0.45">
+    <row r="27" spans="1:15">
       <c r="A27" s="1"/>
       <c r="B27" s="1"/>
       <c r="C27" s="1"/>
@@ -1090,7 +1110,7 @@
       <c r="K27" s="9"/>
       <c r="L27" s="9"/>
     </row>
-    <row r="28" spans="1:12" x14ac:dyDescent="0.45">
+    <row r="28" spans="1:15">
       <c r="A28" s="1"/>
       <c r="B28" s="2" t="s">
         <v>6</v>
@@ -1105,7 +1125,7 @@
       <c r="K28" s="9"/>
       <c r="L28" s="9"/>
     </row>
-    <row r="29" spans="1:12" x14ac:dyDescent="0.45">
+    <row r="29" spans="1:15">
       <c r="A29" s="1"/>
       <c r="B29" s="1"/>
       <c r="C29" s="1"/>
@@ -1121,7 +1141,7 @@
       <c r="K29" s="9"/>
       <c r="L29" s="9"/>
     </row>
-    <row r="30" spans="1:12" x14ac:dyDescent="0.45">
+    <row r="30" spans="1:15">
       <c r="A30" s="1"/>
       <c r="B30" s="1"/>
       <c r="C30" s="1"/>
@@ -1135,7 +1155,7 @@
       <c r="K30" s="9"/>
       <c r="L30" s="9"/>
     </row>
-    <row r="31" spans="1:12" x14ac:dyDescent="0.45">
+    <row r="31" spans="1:15">
       <c r="A31" s="1"/>
       <c r="B31" s="5" t="s">
         <v>8</v>
@@ -1146,7 +1166,7 @@
       <c r="F31" s="1"/>
       <c r="G31" s="1"/>
       <c r="H31" s="19">
-        <f>SUM(A32:G37)</f>
+        <f>SUM(A32:G37, I32:O37)</f>
         <v>0</v>
       </c>
       <c r="I31" s="1"/>
@@ -1154,7 +1174,7 @@
       <c r="K31" s="9"/>
       <c r="L31" s="9"/>
     </row>
-    <row r="32" spans="1:12" x14ac:dyDescent="0.45">
+    <row r="32" spans="1:15">
       <c r="A32" s="20"/>
       <c r="B32" s="21"/>
       <c r="C32" s="20"/>
@@ -1163,12 +1183,14 @@
       <c r="F32" s="21"/>
       <c r="G32" s="20"/>
       <c r="H32" s="1"/>
-      <c r="I32" s="1"/>
+      <c r="I32" s="20"/>
       <c r="J32" s="1"/>
-      <c r="K32" s="9"/>
+      <c r="K32" s="20"/>
       <c r="L32" s="9"/>
-    </row>
-    <row r="33" spans="1:12" x14ac:dyDescent="0.45">
+      <c r="M32" s="20"/>
+      <c r="O32" s="20"/>
+    </row>
+    <row r="33" spans="1:15">
       <c r="A33" s="20"/>
       <c r="B33" s="21"/>
       <c r="C33" s="20"/>
@@ -1177,12 +1199,14 @@
       <c r="F33" s="21"/>
       <c r="G33" s="20"/>
       <c r="H33" s="1"/>
-      <c r="I33" s="1"/>
+      <c r="I33" s="20"/>
       <c r="J33" s="1"/>
-      <c r="K33" s="9"/>
+      <c r="K33" s="20"/>
       <c r="L33" s="9"/>
-    </row>
-    <row r="34" spans="1:12" x14ac:dyDescent="0.45">
+      <c r="M33" s="20"/>
+      <c r="O33" s="20"/>
+    </row>
+    <row r="34" spans="1:15">
       <c r="A34" s="20"/>
       <c r="B34" s="21"/>
       <c r="C34" s="20"/>
@@ -1191,12 +1215,14 @@
       <c r="F34" s="21"/>
       <c r="G34" s="20"/>
       <c r="H34" s="1"/>
-      <c r="I34" s="1"/>
+      <c r="I34" s="20"/>
       <c r="J34" s="1"/>
-      <c r="K34" s="22"/>
+      <c r="K34" s="20"/>
       <c r="L34" s="1"/>
-    </row>
-    <row r="35" spans="1:12" x14ac:dyDescent="0.45">
+      <c r="M34" s="20"/>
+      <c r="O34" s="20"/>
+    </row>
+    <row r="35" spans="1:15">
       <c r="A35" s="20"/>
       <c r="B35" s="21"/>
       <c r="C35" s="20"/>
@@ -1205,12 +1231,14 @@
       <c r="F35" s="21"/>
       <c r="G35" s="20"/>
       <c r="H35" s="1"/>
-      <c r="I35" s="1"/>
+      <c r="I35" s="20"/>
       <c r="J35" s="1"/>
-      <c r="K35" s="21"/>
+      <c r="K35" s="20"/>
       <c r="L35" s="1"/>
-    </row>
-    <row r="36" spans="1:12" x14ac:dyDescent="0.45">
+      <c r="M35" s="20"/>
+      <c r="O35" s="20"/>
+    </row>
+    <row r="36" spans="1:15">
       <c r="A36" s="20"/>
       <c r="B36" s="21"/>
       <c r="C36" s="20"/>
@@ -1218,12 +1246,14 @@
       <c r="E36" s="20"/>
       <c r="F36" s="21"/>
       <c r="G36" s="20"/>
-      <c r="I36" s="1"/>
+      <c r="I36" s="20"/>
       <c r="J36" s="1"/>
-      <c r="K36" s="22"/>
+      <c r="K36" s="20"/>
       <c r="L36" s="1"/>
-    </row>
-    <row r="37" spans="1:12" x14ac:dyDescent="0.45">
+      <c r="M36" s="20"/>
+      <c r="O36" s="20"/>
+    </row>
+    <row r="37" spans="1:15">
       <c r="A37" s="20"/>
       <c r="B37" s="21"/>
       <c r="C37" s="20"/>
@@ -1232,12 +1262,14 @@
       <c r="F37" s="21"/>
       <c r="G37" s="20"/>
       <c r="H37" s="9"/>
-      <c r="I37" s="1"/>
+      <c r="I37" s="20"/>
       <c r="J37" s="1"/>
-      <c r="K37" s="22"/>
+      <c r="K37" s="20"/>
       <c r="L37" s="1"/>
-    </row>
-    <row r="38" spans="1:12" x14ac:dyDescent="0.45">
+      <c r="M37" s="20"/>
+      <c r="O37" s="20"/>
+    </row>
+    <row r="38" spans="1:15">
       <c r="A38" s="9"/>
       <c r="B38" s="9"/>
       <c r="C38" s="1"/>
@@ -1251,7 +1283,7 @@
       <c r="K38" s="22"/>
       <c r="L38" s="1"/>
     </row>
-    <row r="39" spans="1:12" x14ac:dyDescent="0.45">
+    <row r="39" spans="1:15">
       <c r="A39" s="9"/>
       <c r="B39" s="25" t="s">
         <v>9</v>
@@ -1262,7 +1294,7 @@
       <c r="F39" s="1"/>
       <c r="G39" s="9"/>
       <c r="H39" s="26">
-        <f>SUM(A40:G45)</f>
+        <f>SUM(A40:G45, I40:O45)</f>
         <v>0</v>
       </c>
       <c r="I39" s="1"/>
@@ -1270,7 +1302,7 @@
       <c r="K39" s="22"/>
       <c r="L39" s="1"/>
     </row>
-    <row r="40" spans="1:12" x14ac:dyDescent="0.45">
+    <row r="40" spans="1:15">
       <c r="A40" s="20"/>
       <c r="B40" s="21"/>
       <c r="C40" s="20"/>
@@ -1278,12 +1310,14 @@
       <c r="E40" s="20"/>
       <c r="F40" s="21"/>
       <c r="G40" s="20"/>
-      <c r="I40" s="1"/>
+      <c r="I40" s="20"/>
       <c r="J40" s="1"/>
-      <c r="K40" s="22"/>
-      <c r="L40" s="1"/>
-    </row>
-    <row r="41" spans="1:12" x14ac:dyDescent="0.45">
+      <c r="K40" s="20"/>
+      <c r="L40" s="9"/>
+      <c r="M40" s="20"/>
+      <c r="O40" s="20"/>
+    </row>
+    <row r="41" spans="1:15">
       <c r="A41" s="20"/>
       <c r="B41" s="21"/>
       <c r="C41" s="20"/>
@@ -1292,12 +1326,14 @@
       <c r="F41" s="21"/>
       <c r="G41" s="20"/>
       <c r="H41" s="1"/>
-      <c r="I41" s="1"/>
+      <c r="I41" s="20"/>
       <c r="J41" s="1"/>
-      <c r="K41" s="22"/>
-      <c r="L41" s="1"/>
-    </row>
-    <row r="42" spans="1:12" x14ac:dyDescent="0.45">
+      <c r="K41" s="20"/>
+      <c r="L41" s="9"/>
+      <c r="M41" s="20"/>
+      <c r="O41" s="20"/>
+    </row>
+    <row r="42" spans="1:15">
       <c r="A42" s="20"/>
       <c r="B42" s="21"/>
       <c r="C42" s="20"/>
@@ -1306,12 +1342,14 @@
       <c r="F42" s="21"/>
       <c r="G42" s="20"/>
       <c r="H42" s="1"/>
-      <c r="I42" s="1"/>
+      <c r="I42" s="20"/>
       <c r="J42" s="1"/>
-      <c r="K42" s="22"/>
+      <c r="K42" s="20"/>
       <c r="L42" s="1"/>
-    </row>
-    <row r="43" spans="1:12" x14ac:dyDescent="0.45">
+      <c r="M42" s="20"/>
+      <c r="O42" s="20"/>
+    </row>
+    <row r="43" spans="1:15">
       <c r="A43" s="20"/>
       <c r="B43" s="21"/>
       <c r="C43" s="20"/>
@@ -1322,12 +1360,14 @@
       <c r="H43" s="18" t="s">
         <v>10</v>
       </c>
-      <c r="I43" s="1"/>
+      <c r="I43" s="20"/>
       <c r="J43" s="1"/>
-      <c r="K43" s="1"/>
+      <c r="K43" s="20"/>
       <c r="L43" s="1"/>
-    </row>
-    <row r="44" spans="1:12" x14ac:dyDescent="0.45">
+      <c r="M43" s="20"/>
+      <c r="O43" s="20"/>
+    </row>
+    <row r="44" spans="1:15">
       <c r="A44" s="20"/>
       <c r="B44" s="21"/>
       <c r="C44" s="20"/>
@@ -1336,12 +1376,14 @@
       <c r="F44" s="21"/>
       <c r="G44" s="20"/>
       <c r="H44" s="1"/>
-      <c r="I44" s="1"/>
+      <c r="I44" s="20"/>
       <c r="J44" s="1"/>
-      <c r="K44" s="1"/>
+      <c r="K44" s="20"/>
       <c r="L44" s="1"/>
-    </row>
-    <row r="45" spans="1:12" x14ac:dyDescent="0.45">
+      <c r="M44" s="20"/>
+      <c r="O44" s="20"/>
+    </row>
+    <row r="45" spans="1:15">
       <c r="A45" s="20"/>
       <c r="B45" s="21"/>
       <c r="C45" s="20"/>
@@ -1349,10 +1391,14 @@
       <c r="E45" s="20"/>
       <c r="F45" s="21"/>
       <c r="G45" s="20"/>
-      <c r="I45" s="1"/>
+      <c r="I45" s="20"/>
       <c r="J45" s="1"/>
-    </row>
-    <row r="46" spans="1:12" x14ac:dyDescent="0.45">
+      <c r="K45" s="20"/>
+      <c r="L45" s="1"/>
+      <c r="M45" s="20"/>
+      <c r="O45" s="20"/>
+    </row>
+    <row r="46" spans="1:15">
       <c r="A46" s="18"/>
       <c r="B46" s="18"/>
       <c r="C46" s="18"/>
@@ -1360,7 +1406,7 @@
       <c r="I46" s="1"/>
       <c r="J46" s="1"/>
     </row>
-    <row r="47" spans="1:12" x14ac:dyDescent="0.45">
+    <row r="47" spans="1:15">
       <c r="E47" s="2" t="s">
         <v>11</v>
       </c>
@@ -1375,7 +1421,7 @@
       <c r="K47" s="1"/>
       <c r="L47" s="1"/>
     </row>
-    <row r="48" spans="1:12" x14ac:dyDescent="0.45">
+    <row r="48" spans="1:15">
       <c r="E48" s="2" t="s">
         <v>13</v>
       </c>
@@ -1390,7 +1436,7 @@
       <c r="K48" s="1"/>
       <c r="L48" s="1"/>
     </row>
-    <row r="52" spans="9:9" x14ac:dyDescent="0.45">
+    <row r="52" spans="9:9">
       <c r="I52" s="2"/>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Refactor create_conciliation to enhance saldo final calculation and update column definitions for discrepancies
</commit_message>
<xml_diff>
--- a/format.xlsx
+++ b/format.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="29127"/>
-  <workbookPr defaultThemeVersion="202300"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="29318"/>
+  <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/76f1a75cf433d042/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/76f1a75cf433d042/Documentos/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="23" documentId="8_{1658749F-1375-4E6A-A401-979035052B8B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{DE03ED7A-FAD4-4D69-9E9C-5C2E394A84F5}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="8_{3583C0AB-3D2F-42F9-9C2E-D823EE7C4E97}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -18,8 +18,11 @@
   <definedNames>
     <definedName name="_xlnm.Print_Area" localSheetId="0">NOVIEMBRE!$A$1:$H$61</definedName>
   </definedNames>
-  <calcPr calcId="191029"/>
+  <calcPr calcId="191028"/>
   <extLst>
+    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
+      <x15:workbookPr chartTrackingRefBase="1"/>
+    </ext>
     <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
       <xcalcf:calcFeatures>
         <xcalcf:feature name="microsoft.com:RD"/>
@@ -27,6 +30,8 @@
         <xcalcf:feature name="microsoft.com:FV"/>
         <xcalcf:feature name="microsoft.com:CNMTM"/>
         <xcalcf:feature name="microsoft.com:LET_WF"/>
+        <xcalcf:feature name="microsoft.com:LAMBDA_WF"/>
+        <xcalcf:feature name="microsoft.com:ARRAYTEXT_WF"/>
       </xcalcf:calcFeatures>
     </ext>
     <ext xmlns:loext="http://schemas.libreoffice.org/" uri="{7626C862-2A13-11E5-B345-FEFF819CDC9F}">
@@ -57,6 +62,9 @@
     <t>RETIROS (-)</t>
   </si>
   <si>
+    <t>SALDO EN LIBROS</t>
+  </si>
+  <si>
     <t>SALDO EN ESTADO DE CUENTA</t>
   </si>
   <si>
@@ -73,9 +81,6 @@
   </si>
   <si>
     <t>SALDO EN BANCOS</t>
-  </si>
-  <si>
-    <t>SALDO EN LIBROS</t>
   </si>
   <si>
     <t>SOBRANTE</t>
@@ -222,7 +227,7 @@
     <xf numFmtId="164" fontId="10" fillId="0" borderId="0" applyBorder="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="10" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="36">
+  <cellXfs count="35">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="4"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="4" applyFont="1"/>
@@ -268,7 +273,6 @@
     <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="49" fontId="4" fillId="0" borderId="0" xfId="3" applyNumberFormat="1" applyFont="1" applyBorder="1" applyProtection="1"/>
     <xf numFmtId="164" fontId="1" fillId="0" borderId="1" xfId="3" applyFont="1" applyBorder="1" applyProtection="1"/>
-    <xf numFmtId="165" fontId="10" fillId="0" borderId="0" xfId="4" applyNumberFormat="1"/>
     <xf numFmtId="164" fontId="1" fillId="0" borderId="2" xfId="1" applyFont="1" applyBorder="1" applyProtection="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="4" applyFont="1" applyBorder="1"/>
     <xf numFmtId="166" fontId="8" fillId="0" borderId="0" xfId="2" applyFont="1" applyBorder="1" applyProtection="1"/>
@@ -279,9 +283,9 @@
     <xf numFmtId="165" fontId="4" fillId="0" borderId="0" xfId="4" applyNumberFormat="1" applyFont="1"/>
   </cellXfs>
   <cellStyles count="5">
+    <cellStyle name="Comma" xfId="1" builtinId="3"/>
     <cellStyle name="Comma 2" xfId="3" xr:uid="{00000000-0005-0000-0000-000006000000}"/>
-    <cellStyle name="Millares" xfId="1" builtinId="3"/>
-    <cellStyle name="Moneda" xfId="2" builtinId="4"/>
+    <cellStyle name="Currency" xfId="2" builtinId="4"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
     <cellStyle name="Normal 2" xfId="4" xr:uid="{00000000-0005-0000-0000-000007000000}"/>
   </cellStyles>
@@ -686,21 +690,21 @@
   <sheetPr>
     <tabColor rgb="FF7030A0"/>
   </sheetPr>
-  <dimension ref="A1:O52"/>
+  <dimension ref="A1:Z52"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="53" zoomScaleNormal="160" workbookViewId="0">
-      <selection activeCell="I28" sqref="I28"/>
+    <sheetView tabSelected="1" topLeftCell="A4" zoomScale="54" zoomScaleNormal="160" workbookViewId="0">
+      <selection activeCell="H39" sqref="H39"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="11.296875" defaultRowHeight="13.8"/>
+  <sheetFormatPr defaultColWidth="11.28515625" defaultRowHeight="13.9"/>
   <cols>
-    <col min="4" max="4" width="7.5" customWidth="1"/>
-    <col min="5" max="5" width="12.296875" customWidth="1"/>
-    <col min="8" max="8" width="13.796875" customWidth="1"/>
-    <col min="9" max="9" width="12.296875" customWidth="1"/>
+    <col min="4" max="4" width="7.42578125" customWidth="1"/>
+    <col min="5" max="5" width="12.28515625" customWidth="1"/>
+    <col min="8" max="8" width="13.85546875" customWidth="1"/>
+    <col min="9" max="9" width="12.28515625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:15">
+    <row r="1" spans="1:26">
       <c r="A1" s="1"/>
       <c r="B1" s="2" t="s">
         <v>0</v>
@@ -716,7 +720,7 @@
       <c r="K1" s="1"/>
       <c r="L1" s="1"/>
     </row>
-    <row r="2" spans="1:15">
+    <row r="2" spans="1:26">
       <c r="A2" s="1"/>
       <c r="B2" s="2" t="s">
         <v>1</v>
@@ -732,7 +736,7 @@
       <c r="K2" s="1"/>
       <c r="L2" s="1"/>
     </row>
-    <row r="3" spans="1:15">
+    <row r="3" spans="1:26">
       <c r="A3" s="1"/>
       <c r="B3" s="2" t="s">
         <v>2</v>
@@ -748,10 +752,10 @@
       <c r="K3" s="1"/>
       <c r="L3" s="1"/>
     </row>
-    <row r="4" spans="1:15">
+    <row r="4" spans="1:26">
       <c r="B4" s="2"/>
     </row>
-    <row r="5" spans="1:15">
+    <row r="5" spans="1:26">
       <c r="A5" s="1"/>
       <c r="B5" s="1"/>
       <c r="C5" s="1"/>
@@ -765,7 +769,7 @@
       <c r="K5" s="9"/>
       <c r="L5" s="9"/>
     </row>
-    <row r="6" spans="1:15">
+    <row r="6" spans="1:26">
       <c r="A6" s="1"/>
       <c r="B6" s="10" t="s">
         <v>3</v>
@@ -781,7 +785,7 @@
       <c r="K6" s="9"/>
       <c r="L6" s="9"/>
     </row>
-    <row r="7" spans="1:15">
+    <row r="7" spans="1:26">
       <c r="A7" s="1"/>
       <c r="B7" s="1"/>
       <c r="C7" s="14"/>
@@ -795,7 +799,7 @@
       <c r="K7" s="9"/>
       <c r="L7" s="9"/>
     </row>
-    <row r="8" spans="1:15">
+    <row r="8" spans="1:26">
       <c r="A8" s="1"/>
       <c r="B8" s="1"/>
       <c r="C8" s="1"/>
@@ -809,7 +813,7 @@
       <c r="K8" s="9"/>
       <c r="L8" s="9"/>
     </row>
-    <row r="9" spans="1:15">
+    <row r="9" spans="1:26">
       <c r="A9" s="1"/>
       <c r="B9" s="15" t="s">
         <v>4</v>
@@ -820,7 +824,7 @@
       <c r="F9" s="17"/>
       <c r="G9" s="18"/>
       <c r="H9" s="19">
-        <f>SUM(A10:G15, I10:O15)</f>
+        <f>SUM(A10:G15, I10:Z15)</f>
         <v>0</v>
       </c>
       <c r="I9" s="1"/>
@@ -828,7 +832,7 @@
       <c r="K9" s="9"/>
       <c r="L9" s="9"/>
     </row>
-    <row r="10" spans="1:15">
+    <row r="10" spans="1:26">
       <c r="A10" s="20"/>
       <c r="B10" s="21"/>
       <c r="C10" s="20"/>
@@ -838,14 +842,24 @@
       <c r="G10" s="20"/>
       <c r="H10" s="23"/>
       <c r="I10" s="20"/>
-      <c r="J10" s="1"/>
+      <c r="J10" s="21"/>
       <c r="K10" s="20"/>
-      <c r="L10" s="5"/>
+      <c r="L10" s="21"/>
       <c r="M10" s="20"/>
-      <c r="N10" s="1"/>
+      <c r="N10" s="21"/>
       <c r="O10" s="20"/>
-    </row>
-    <row r="11" spans="1:15">
+      <c r="Q10" s="20"/>
+      <c r="R10" s="21"/>
+      <c r="S10" s="20"/>
+      <c r="T10" s="21"/>
+      <c r="U10" s="20"/>
+      <c r="V10" s="21"/>
+      <c r="W10" s="20"/>
+      <c r="X10" s="21"/>
+      <c r="Y10" s="20"/>
+      <c r="Z10" s="21"/>
+    </row>
+    <row r="11" spans="1:26">
       <c r="A11" s="20"/>
       <c r="B11" s="21"/>
       <c r="C11" s="20"/>
@@ -854,14 +868,24 @@
       <c r="F11" s="21"/>
       <c r="G11" s="20"/>
       <c r="I11" s="20"/>
-      <c r="J11" s="1"/>
+      <c r="J11" s="21"/>
       <c r="K11" s="20"/>
-      <c r="L11" s="2"/>
+      <c r="L11" s="21"/>
       <c r="M11" s="20"/>
-      <c r="N11" s="2"/>
+      <c r="N11" s="21"/>
       <c r="O11" s="20"/>
-    </row>
-    <row r="12" spans="1:15">
+      <c r="Q11" s="20"/>
+      <c r="R11" s="21"/>
+      <c r="S11" s="20"/>
+      <c r="T11" s="21"/>
+      <c r="U11" s="20"/>
+      <c r="V11" s="21"/>
+      <c r="W11" s="20"/>
+      <c r="X11" s="21"/>
+      <c r="Y11" s="20"/>
+      <c r="Z11" s="21"/>
+    </row>
+    <row r="12" spans="1:26">
       <c r="A12" s="20"/>
       <c r="B12" s="21"/>
       <c r="C12" s="20"/>
@@ -871,13 +895,24 @@
       <c r="G12" s="20"/>
       <c r="H12" s="1"/>
       <c r="I12" s="20"/>
-      <c r="J12" s="1"/>
+      <c r="J12" s="21"/>
       <c r="K12" s="20"/>
-      <c r="L12" s="9"/>
+      <c r="L12" s="21"/>
       <c r="M12" s="20"/>
+      <c r="N12" s="21"/>
       <c r="O12" s="20"/>
-    </row>
-    <row r="13" spans="1:15">
+      <c r="Q12" s="20"/>
+      <c r="R12" s="21"/>
+      <c r="S12" s="20"/>
+      <c r="T12" s="21"/>
+      <c r="U12" s="20"/>
+      <c r="V12" s="21"/>
+      <c r="W12" s="20"/>
+      <c r="X12" s="21"/>
+      <c r="Y12" s="20"/>
+      <c r="Z12" s="21"/>
+    </row>
+    <row r="13" spans="1:26">
       <c r="A13" s="20"/>
       <c r="B13" s="21"/>
       <c r="C13" s="20"/>
@@ -887,13 +922,24 @@
       <c r="G13" s="20"/>
       <c r="H13" s="1"/>
       <c r="I13" s="20"/>
-      <c r="J13" s="1"/>
+      <c r="J13" s="21"/>
       <c r="K13" s="20"/>
-      <c r="L13" s="9"/>
+      <c r="L13" s="21"/>
       <c r="M13" s="20"/>
+      <c r="N13" s="21"/>
       <c r="O13" s="20"/>
-    </row>
-    <row r="14" spans="1:15">
+      <c r="Q13" s="20"/>
+      <c r="R13" s="21"/>
+      <c r="S13" s="20"/>
+      <c r="T13" s="21"/>
+      <c r="U13" s="20"/>
+      <c r="V13" s="21"/>
+      <c r="W13" s="20"/>
+      <c r="X13" s="21"/>
+      <c r="Y13" s="20"/>
+      <c r="Z13" s="21"/>
+    </row>
+    <row r="14" spans="1:26">
       <c r="A14" s="20"/>
       <c r="B14" s="21"/>
       <c r="C14" s="20"/>
@@ -903,13 +949,24 @@
       <c r="G14" s="20"/>
       <c r="H14" s="1"/>
       <c r="I14" s="20"/>
-      <c r="J14" s="1"/>
+      <c r="J14" s="21"/>
       <c r="K14" s="20"/>
-      <c r="L14" s="9"/>
+      <c r="L14" s="21"/>
       <c r="M14" s="20"/>
+      <c r="N14" s="21"/>
       <c r="O14" s="20"/>
-    </row>
-    <row r="15" spans="1:15">
+      <c r="Q14" s="20"/>
+      <c r="R14" s="21"/>
+      <c r="S14" s="20"/>
+      <c r="T14" s="21"/>
+      <c r="U14" s="20"/>
+      <c r="V14" s="21"/>
+      <c r="W14" s="20"/>
+      <c r="X14" s="21"/>
+      <c r="Y14" s="20"/>
+      <c r="Z14" s="21"/>
+    </row>
+    <row r="15" spans="1:26">
       <c r="A15" s="20"/>
       <c r="B15" s="21"/>
       <c r="C15" s="20"/>
@@ -919,13 +976,24 @@
       <c r="G15" s="20"/>
       <c r="H15" s="1"/>
       <c r="I15" s="20"/>
-      <c r="J15" s="1"/>
+      <c r="J15" s="21"/>
       <c r="K15" s="20"/>
-      <c r="L15" s="9"/>
+      <c r="L15" s="21"/>
       <c r="M15" s="20"/>
+      <c r="N15" s="21"/>
       <c r="O15" s="20"/>
-    </row>
-    <row r="16" spans="1:15">
+      <c r="Q15" s="20"/>
+      <c r="R15" s="21"/>
+      <c r="S15" s="20"/>
+      <c r="T15" s="21"/>
+      <c r="U15" s="20"/>
+      <c r="V15" s="21"/>
+      <c r="W15" s="20"/>
+      <c r="X15" s="21"/>
+      <c r="Y15" s="20"/>
+      <c r="Z15" s="21"/>
+    </row>
+    <row r="16" spans="1:26">
       <c r="A16" s="21"/>
       <c r="B16" s="24"/>
       <c r="C16" s="21"/>
@@ -939,7 +1007,7 @@
       <c r="K16" s="9"/>
       <c r="L16" s="9"/>
     </row>
-    <row r="17" spans="1:15">
+    <row r="17" spans="1:26">
       <c r="A17" s="21"/>
       <c r="B17" s="25" t="s">
         <v>5</v>
@@ -950,7 +1018,7 @@
       <c r="F17" s="2"/>
       <c r="G17" s="9"/>
       <c r="H17" s="26">
-        <f>SUM(A18:G23, I18:O23)</f>
+        <f>SUM(A18:G23, I18:Z23)</f>
         <v>0</v>
       </c>
       <c r="I17" s="1"/>
@@ -958,7 +1026,7 @@
       <c r="K17" s="9"/>
       <c r="L17" s="9"/>
     </row>
-    <row r="18" spans="1:15">
+    <row r="18" spans="1:26">
       <c r="A18" s="20"/>
       <c r="B18" s="21"/>
       <c r="C18" s="20"/>
@@ -966,16 +1034,26 @@
       <c r="E18" s="20"/>
       <c r="F18" s="21"/>
       <c r="G18" s="20"/>
-      <c r="H18" s="1"/>
+      <c r="H18" s="23"/>
       <c r="I18" s="20"/>
-      <c r="J18" s="1"/>
+      <c r="J18" s="21"/>
       <c r="K18" s="20"/>
-      <c r="L18" s="5"/>
+      <c r="L18" s="21"/>
       <c r="M18" s="20"/>
-      <c r="N18" s="1"/>
+      <c r="N18" s="21"/>
       <c r="O18" s="20"/>
-    </row>
-    <row r="19" spans="1:15">
+      <c r="Q18" s="20"/>
+      <c r="R18" s="21"/>
+      <c r="S18" s="20"/>
+      <c r="T18" s="21"/>
+      <c r="U18" s="20"/>
+      <c r="V18" s="21"/>
+      <c r="W18" s="20"/>
+      <c r="X18" s="21"/>
+      <c r="Y18" s="20"/>
+      <c r="Z18" s="21"/>
+    </row>
+    <row r="19" spans="1:26">
       <c r="A19" s="20"/>
       <c r="B19" s="21"/>
       <c r="C19" s="20"/>
@@ -983,16 +1061,25 @@
       <c r="E19" s="20"/>
       <c r="F19" s="21"/>
       <c r="G19" s="20"/>
-      <c r="H19" s="1"/>
       <c r="I19" s="20"/>
-      <c r="J19" s="1"/>
+      <c r="J19" s="21"/>
       <c r="K19" s="20"/>
-      <c r="L19" s="2"/>
+      <c r="L19" s="21"/>
       <c r="M19" s="20"/>
-      <c r="N19" s="2"/>
+      <c r="N19" s="21"/>
       <c r="O19" s="20"/>
-    </row>
-    <row r="20" spans="1:15">
+      <c r="Q19" s="20"/>
+      <c r="R19" s="21"/>
+      <c r="S19" s="20"/>
+      <c r="T19" s="21"/>
+      <c r="U19" s="20"/>
+      <c r="V19" s="21"/>
+      <c r="W19" s="20"/>
+      <c r="X19" s="21"/>
+      <c r="Y19" s="20"/>
+      <c r="Z19" s="21"/>
+    </row>
+    <row r="20" spans="1:26">
       <c r="A20" s="20"/>
       <c r="B20" s="21"/>
       <c r="C20" s="20"/>
@@ -1002,13 +1089,24 @@
       <c r="G20" s="20"/>
       <c r="H20" s="1"/>
       <c r="I20" s="20"/>
-      <c r="J20" s="1"/>
+      <c r="J20" s="21"/>
       <c r="K20" s="20"/>
-      <c r="L20" s="9"/>
+      <c r="L20" s="21"/>
       <c r="M20" s="20"/>
+      <c r="N20" s="21"/>
       <c r="O20" s="20"/>
-    </row>
-    <row r="21" spans="1:15">
+      <c r="Q20" s="20"/>
+      <c r="R20" s="21"/>
+      <c r="S20" s="20"/>
+      <c r="T20" s="21"/>
+      <c r="U20" s="20"/>
+      <c r="V20" s="21"/>
+      <c r="W20" s="20"/>
+      <c r="X20" s="21"/>
+      <c r="Y20" s="20"/>
+      <c r="Z20" s="21"/>
+    </row>
+    <row r="21" spans="1:26">
       <c r="A21" s="20"/>
       <c r="B21" s="21"/>
       <c r="C21" s="20"/>
@@ -1018,13 +1116,24 @@
       <c r="G21" s="20"/>
       <c r="H21" s="1"/>
       <c r="I21" s="20"/>
-      <c r="J21" s="1"/>
+      <c r="J21" s="21"/>
       <c r="K21" s="20"/>
-      <c r="L21" s="9"/>
+      <c r="L21" s="21"/>
       <c r="M21" s="20"/>
+      <c r="N21" s="21"/>
       <c r="O21" s="20"/>
-    </row>
-    <row r="22" spans="1:15">
+      <c r="Q21" s="20"/>
+      <c r="R21" s="21"/>
+      <c r="S21" s="20"/>
+      <c r="T21" s="21"/>
+      <c r="U21" s="20"/>
+      <c r="V21" s="21"/>
+      <c r="W21" s="20"/>
+      <c r="X21" s="21"/>
+      <c r="Y21" s="20"/>
+      <c r="Z21" s="21"/>
+    </row>
+    <row r="22" spans="1:26">
       <c r="A22" s="20"/>
       <c r="B22" s="21"/>
       <c r="C22" s="20"/>
@@ -1032,14 +1141,26 @@
       <c r="E22" s="20"/>
       <c r="F22" s="21"/>
       <c r="G22" s="20"/>
+      <c r="H22" s="1"/>
       <c r="I22" s="20"/>
-      <c r="J22" s="1"/>
+      <c r="J22" s="21"/>
       <c r="K22" s="20"/>
-      <c r="L22" s="9"/>
+      <c r="L22" s="21"/>
       <c r="M22" s="20"/>
+      <c r="N22" s="21"/>
       <c r="O22" s="20"/>
-    </row>
-    <row r="23" spans="1:15">
+      <c r="Q22" s="20"/>
+      <c r="R22" s="21"/>
+      <c r="S22" s="20"/>
+      <c r="T22" s="21"/>
+      <c r="U22" s="20"/>
+      <c r="V22" s="21"/>
+      <c r="W22" s="20"/>
+      <c r="X22" s="21"/>
+      <c r="Y22" s="20"/>
+      <c r="Z22" s="21"/>
+    </row>
+    <row r="23" spans="1:26">
       <c r="A23" s="20"/>
       <c r="B23" s="21"/>
       <c r="C23" s="20"/>
@@ -1047,15 +1168,26 @@
       <c r="E23" s="20"/>
       <c r="F23" s="21"/>
       <c r="G23" s="20"/>
-      <c r="H23" s="27"/>
+      <c r="H23" s="1"/>
       <c r="I23" s="20"/>
-      <c r="J23" s="1"/>
+      <c r="J23" s="21"/>
       <c r="K23" s="20"/>
-      <c r="L23" s="9"/>
+      <c r="L23" s="21"/>
       <c r="M23" s="20"/>
+      <c r="N23" s="21"/>
       <c r="O23" s="20"/>
-    </row>
-    <row r="24" spans="1:15">
+      <c r="Q23" s="20"/>
+      <c r="R23" s="21"/>
+      <c r="S23" s="20"/>
+      <c r="T23" s="21"/>
+      <c r="U23" s="20"/>
+      <c r="V23" s="21"/>
+      <c r="W23" s="20"/>
+      <c r="X23" s="21"/>
+      <c r="Y23" s="20"/>
+      <c r="Z23" s="21"/>
+    </row>
+    <row r="24" spans="1:26">
       <c r="A24" s="21"/>
       <c r="B24" s="21"/>
       <c r="C24" s="21"/>
@@ -1068,9 +1200,9 @@
       <c r="K24" s="9"/>
       <c r="L24" s="9"/>
     </row>
-    <row r="25" spans="1:15">
+    <row r="25" spans="1:26">
       <c r="E25" s="2" t="s">
-        <v>12</v>
+        <v>6</v>
       </c>
       <c r="G25" s="2"/>
       <c r="H25" s="12">
@@ -1082,21 +1214,21 @@
       <c r="K25" s="9"/>
       <c r="L25" s="9"/>
     </row>
-    <row r="26" spans="1:15">
-      <c r="A26" s="28"/>
-      <c r="B26" s="28"/>
-      <c r="C26" s="28"/>
-      <c r="D26" s="28"/>
-      <c r="E26" s="29"/>
-      <c r="F26" s="29"/>
-      <c r="G26" s="29"/>
-      <c r="H26" s="29"/>
+    <row r="26" spans="1:26">
+      <c r="A26" s="27"/>
+      <c r="B26" s="27"/>
+      <c r="C26" s="27"/>
+      <c r="D26" s="27"/>
+      <c r="E26" s="28"/>
+      <c r="F26" s="28"/>
+      <c r="G26" s="28"/>
+      <c r="H26" s="28"/>
       <c r="I26" s="1"/>
       <c r="J26" s="13"/>
       <c r="K26" s="9"/>
       <c r="L26" s="9"/>
     </row>
-    <row r="27" spans="1:15">
+    <row r="27" spans="1:26">
       <c r="A27" s="1"/>
       <c r="B27" s="1"/>
       <c r="C27" s="1"/>
@@ -1105,19 +1237,19 @@
       <c r="F27" s="1"/>
       <c r="G27" s="1"/>
       <c r="H27" s="1"/>
-      <c r="I27" s="30"/>
+      <c r="I27" s="29"/>
       <c r="J27" s="13"/>
       <c r="K27" s="9"/>
       <c r="L27" s="9"/>
     </row>
-    <row r="28" spans="1:15">
+    <row r="28" spans="1:26">
       <c r="A28" s="1"/>
       <c r="B28" s="2" t="s">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="C28" s="2"/>
-      <c r="E28" s="31"/>
-      <c r="F28" s="32"/>
+      <c r="E28" s="30"/>
+      <c r="F28" s="31"/>
       <c r="G28" s="21"/>
       <c r="H28" s="12"/>
       <c r="I28" s="1"/>
@@ -1125,7 +1257,7 @@
       <c r="K28" s="9"/>
       <c r="L28" s="9"/>
     </row>
-    <row r="29" spans="1:15">
+    <row r="29" spans="1:26">
       <c r="A29" s="1"/>
       <c r="B29" s="1"/>
       <c r="C29" s="1"/>
@@ -1134,14 +1266,14 @@
       <c r="F29" s="1"/>
       <c r="G29" s="1"/>
       <c r="H29" s="2" t="s">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="I29" s="1"/>
       <c r="J29" s="1"/>
       <c r="K29" s="9"/>
       <c r="L29" s="9"/>
     </row>
-    <row r="30" spans="1:15">
+    <row r="30" spans="1:26">
       <c r="A30" s="1"/>
       <c r="B30" s="1"/>
       <c r="C30" s="1"/>
@@ -1155,10 +1287,10 @@
       <c r="K30" s="9"/>
       <c r="L30" s="9"/>
     </row>
-    <row r="31" spans="1:15">
+    <row r="31" spans="1:26">
       <c r="A31" s="1"/>
       <c r="B31" s="5" t="s">
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="C31" s="5"/>
       <c r="D31" s="5"/>
@@ -1166,7 +1298,7 @@
       <c r="F31" s="1"/>
       <c r="G31" s="1"/>
       <c r="H31" s="19">
-        <f>SUM(A32:G37, I32:O37)</f>
+        <f>SUM(A32:G37, I32:Z37)</f>
         <v>0</v>
       </c>
       <c r="I31" s="1"/>
@@ -1174,7 +1306,7 @@
       <c r="K31" s="9"/>
       <c r="L31" s="9"/>
     </row>
-    <row r="32" spans="1:15">
+    <row r="32" spans="1:26">
       <c r="A32" s="20"/>
       <c r="B32" s="21"/>
       <c r="C32" s="20"/>
@@ -1182,15 +1314,26 @@
       <c r="E32" s="20"/>
       <c r="F32" s="21"/>
       <c r="G32" s="20"/>
-      <c r="H32" s="1"/>
+      <c r="H32" s="23"/>
       <c r="I32" s="20"/>
-      <c r="J32" s="1"/>
+      <c r="J32" s="21"/>
       <c r="K32" s="20"/>
-      <c r="L32" s="9"/>
+      <c r="L32" s="21"/>
       <c r="M32" s="20"/>
+      <c r="N32" s="21"/>
       <c r="O32" s="20"/>
-    </row>
-    <row r="33" spans="1:15">
+      <c r="Q32" s="20"/>
+      <c r="R32" s="21"/>
+      <c r="S32" s="20"/>
+      <c r="T32" s="21"/>
+      <c r="U32" s="20"/>
+      <c r="V32" s="21"/>
+      <c r="W32" s="20"/>
+      <c r="X32" s="21"/>
+      <c r="Y32" s="20"/>
+      <c r="Z32" s="21"/>
+    </row>
+    <row r="33" spans="1:26">
       <c r="A33" s="20"/>
       <c r="B33" s="21"/>
       <c r="C33" s="20"/>
@@ -1198,15 +1341,25 @@
       <c r="E33" s="20"/>
       <c r="F33" s="21"/>
       <c r="G33" s="20"/>
-      <c r="H33" s="1"/>
       <c r="I33" s="20"/>
-      <c r="J33" s="1"/>
+      <c r="J33" s="21"/>
       <c r="K33" s="20"/>
-      <c r="L33" s="9"/>
+      <c r="L33" s="21"/>
       <c r="M33" s="20"/>
+      <c r="N33" s="21"/>
       <c r="O33" s="20"/>
-    </row>
-    <row r="34" spans="1:15">
+      <c r="Q33" s="20"/>
+      <c r="R33" s="21"/>
+      <c r="S33" s="20"/>
+      <c r="T33" s="21"/>
+      <c r="U33" s="20"/>
+      <c r="V33" s="21"/>
+      <c r="W33" s="20"/>
+      <c r="X33" s="21"/>
+      <c r="Y33" s="20"/>
+      <c r="Z33" s="21"/>
+    </row>
+    <row r="34" spans="1:26">
       <c r="A34" s="20"/>
       <c r="B34" s="21"/>
       <c r="C34" s="20"/>
@@ -1216,13 +1369,24 @@
       <c r="G34" s="20"/>
       <c r="H34" s="1"/>
       <c r="I34" s="20"/>
-      <c r="J34" s="1"/>
+      <c r="J34" s="21"/>
       <c r="K34" s="20"/>
-      <c r="L34" s="1"/>
+      <c r="L34" s="21"/>
       <c r="M34" s="20"/>
+      <c r="N34" s="21"/>
       <c r="O34" s="20"/>
-    </row>
-    <row r="35" spans="1:15">
+      <c r="Q34" s="20"/>
+      <c r="R34" s="21"/>
+      <c r="S34" s="20"/>
+      <c r="T34" s="21"/>
+      <c r="U34" s="20"/>
+      <c r="V34" s="21"/>
+      <c r="W34" s="20"/>
+      <c r="X34" s="21"/>
+      <c r="Y34" s="20"/>
+      <c r="Z34" s="21"/>
+    </row>
+    <row r="35" spans="1:26">
       <c r="A35" s="20"/>
       <c r="B35" s="21"/>
       <c r="C35" s="20"/>
@@ -1232,13 +1396,24 @@
       <c r="G35" s="20"/>
       <c r="H35" s="1"/>
       <c r="I35" s="20"/>
-      <c r="J35" s="1"/>
+      <c r="J35" s="21"/>
       <c r="K35" s="20"/>
-      <c r="L35" s="1"/>
+      <c r="L35" s="21"/>
       <c r="M35" s="20"/>
+      <c r="N35" s="21"/>
       <c r="O35" s="20"/>
-    </row>
-    <row r="36" spans="1:15">
+      <c r="Q35" s="20"/>
+      <c r="R35" s="21"/>
+      <c r="S35" s="20"/>
+      <c r="T35" s="21"/>
+      <c r="U35" s="20"/>
+      <c r="V35" s="21"/>
+      <c r="W35" s="20"/>
+      <c r="X35" s="21"/>
+      <c r="Y35" s="20"/>
+      <c r="Z35" s="21"/>
+    </row>
+    <row r="36" spans="1:26">
       <c r="A36" s="20"/>
       <c r="B36" s="21"/>
       <c r="C36" s="20"/>
@@ -1246,14 +1421,26 @@
       <c r="E36" s="20"/>
       <c r="F36" s="21"/>
       <c r="G36" s="20"/>
+      <c r="H36" s="1"/>
       <c r="I36" s="20"/>
-      <c r="J36" s="1"/>
+      <c r="J36" s="21"/>
       <c r="K36" s="20"/>
-      <c r="L36" s="1"/>
+      <c r="L36" s="21"/>
       <c r="M36" s="20"/>
+      <c r="N36" s="21"/>
       <c r="O36" s="20"/>
-    </row>
-    <row r="37" spans="1:15">
+      <c r="Q36" s="20"/>
+      <c r="R36" s="21"/>
+      <c r="S36" s="20"/>
+      <c r="T36" s="21"/>
+      <c r="U36" s="20"/>
+      <c r="V36" s="21"/>
+      <c r="W36" s="20"/>
+      <c r="X36" s="21"/>
+      <c r="Y36" s="20"/>
+      <c r="Z36" s="21"/>
+    </row>
+    <row r="37" spans="1:26">
       <c r="A37" s="20"/>
       <c r="B37" s="21"/>
       <c r="C37" s="20"/>
@@ -1261,15 +1448,26 @@
       <c r="E37" s="20"/>
       <c r="F37" s="21"/>
       <c r="G37" s="20"/>
-      <c r="H37" s="9"/>
+      <c r="H37" s="1"/>
       <c r="I37" s="20"/>
-      <c r="J37" s="1"/>
+      <c r="J37" s="21"/>
       <c r="K37" s="20"/>
-      <c r="L37" s="1"/>
+      <c r="L37" s="21"/>
       <c r="M37" s="20"/>
+      <c r="N37" s="21"/>
       <c r="O37" s="20"/>
-    </row>
-    <row r="38" spans="1:15">
+      <c r="Q37" s="20"/>
+      <c r="R37" s="21"/>
+      <c r="S37" s="20"/>
+      <c r="T37" s="21"/>
+      <c r="U37" s="20"/>
+      <c r="V37" s="21"/>
+      <c r="W37" s="20"/>
+      <c r="X37" s="21"/>
+      <c r="Y37" s="20"/>
+      <c r="Z37" s="21"/>
+    </row>
+    <row r="38" spans="1:26">
       <c r="A38" s="9"/>
       <c r="B38" s="9"/>
       <c r="C38" s="1"/>
@@ -1283,18 +1481,18 @@
       <c r="K38" s="22"/>
       <c r="L38" s="1"/>
     </row>
-    <row r="39" spans="1:15">
+    <row r="39" spans="1:26">
       <c r="A39" s="9"/>
       <c r="B39" s="25" t="s">
-        <v>9</v>
-      </c>
-      <c r="C39" s="33"/>
-      <c r="D39" s="33"/>
+        <v>10</v>
+      </c>
+      <c r="C39" s="32"/>
+      <c r="D39" s="32"/>
       <c r="E39" s="2"/>
       <c r="F39" s="1"/>
       <c r="G39" s="9"/>
       <c r="H39" s="26">
-        <f>SUM(A40:G45, I40:O45)</f>
+        <f>SUM(A40:G45, I40:Z45)</f>
         <v>0</v>
       </c>
       <c r="I39" s="1"/>
@@ -1302,7 +1500,7 @@
       <c r="K39" s="22"/>
       <c r="L39" s="1"/>
     </row>
-    <row r="40" spans="1:15">
+    <row r="40" spans="1:26">
       <c r="A40" s="20"/>
       <c r="B40" s="21"/>
       <c r="C40" s="20"/>
@@ -1310,14 +1508,26 @@
       <c r="E40" s="20"/>
       <c r="F40" s="21"/>
       <c r="G40" s="20"/>
+      <c r="H40" s="23"/>
       <c r="I40" s="20"/>
-      <c r="J40" s="1"/>
+      <c r="J40" s="21"/>
       <c r="K40" s="20"/>
-      <c r="L40" s="9"/>
+      <c r="L40" s="21"/>
       <c r="M40" s="20"/>
+      <c r="N40" s="21"/>
       <c r="O40" s="20"/>
-    </row>
-    <row r="41" spans="1:15">
+      <c r="Q40" s="20"/>
+      <c r="R40" s="21"/>
+      <c r="S40" s="20"/>
+      <c r="T40" s="21"/>
+      <c r="U40" s="20"/>
+      <c r="V40" s="21"/>
+      <c r="W40" s="20"/>
+      <c r="X40" s="21"/>
+      <c r="Y40" s="20"/>
+      <c r="Z40" s="21"/>
+    </row>
+    <row r="41" spans="1:26">
       <c r="A41" s="20"/>
       <c r="B41" s="21"/>
       <c r="C41" s="20"/>
@@ -1325,15 +1535,25 @@
       <c r="E41" s="20"/>
       <c r="F41" s="21"/>
       <c r="G41" s="20"/>
-      <c r="H41" s="1"/>
       <c r="I41" s="20"/>
-      <c r="J41" s="1"/>
+      <c r="J41" s="21"/>
       <c r="K41" s="20"/>
-      <c r="L41" s="9"/>
+      <c r="L41" s="21"/>
       <c r="M41" s="20"/>
+      <c r="N41" s="21"/>
       <c r="O41" s="20"/>
-    </row>
-    <row r="42" spans="1:15">
+      <c r="Q41" s="20"/>
+      <c r="R41" s="21"/>
+      <c r="S41" s="20"/>
+      <c r="T41" s="21"/>
+      <c r="U41" s="20"/>
+      <c r="V41" s="21"/>
+      <c r="W41" s="20"/>
+      <c r="X41" s="21"/>
+      <c r="Y41" s="20"/>
+      <c r="Z41" s="21"/>
+    </row>
+    <row r="42" spans="1:26">
       <c r="A42" s="20"/>
       <c r="B42" s="21"/>
       <c r="C42" s="20"/>
@@ -1343,13 +1563,24 @@
       <c r="G42" s="20"/>
       <c r="H42" s="1"/>
       <c r="I42" s="20"/>
-      <c r="J42" s="1"/>
+      <c r="J42" s="21"/>
       <c r="K42" s="20"/>
-      <c r="L42" s="1"/>
+      <c r="L42" s="21"/>
       <c r="M42" s="20"/>
+      <c r="N42" s="21"/>
       <c r="O42" s="20"/>
-    </row>
-    <row r="43" spans="1:15">
+      <c r="Q42" s="20"/>
+      <c r="R42" s="21"/>
+      <c r="S42" s="20"/>
+      <c r="T42" s="21"/>
+      <c r="U42" s="20"/>
+      <c r="V42" s="21"/>
+      <c r="W42" s="20"/>
+      <c r="X42" s="21"/>
+      <c r="Y42" s="20"/>
+      <c r="Z42" s="21"/>
+    </row>
+    <row r="43" spans="1:26">
       <c r="A43" s="20"/>
       <c r="B43" s="21"/>
       <c r="C43" s="20"/>
@@ -1357,17 +1588,28 @@
       <c r="E43" s="20"/>
       <c r="F43" s="21"/>
       <c r="G43" s="20"/>
-      <c r="H43" s="18" t="s">
-        <v>10</v>
+      <c r="H43" s="1" t="s">
+        <v>11</v>
       </c>
       <c r="I43" s="20"/>
-      <c r="J43" s="1"/>
+      <c r="J43" s="21"/>
       <c r="K43" s="20"/>
-      <c r="L43" s="1"/>
+      <c r="L43" s="21"/>
       <c r="M43" s="20"/>
+      <c r="N43" s="21"/>
       <c r="O43" s="20"/>
-    </row>
-    <row r="44" spans="1:15">
+      <c r="Q43" s="20"/>
+      <c r="R43" s="21"/>
+      <c r="S43" s="20"/>
+      <c r="T43" s="21"/>
+      <c r="U43" s="20"/>
+      <c r="V43" s="21"/>
+      <c r="W43" s="20"/>
+      <c r="X43" s="21"/>
+      <c r="Y43" s="20"/>
+      <c r="Z43" s="21"/>
+    </row>
+    <row r="44" spans="1:26">
       <c r="A44" s="20"/>
       <c r="B44" s="21"/>
       <c r="C44" s="20"/>
@@ -1377,13 +1619,24 @@
       <c r="G44" s="20"/>
       <c r="H44" s="1"/>
       <c r="I44" s="20"/>
-      <c r="J44" s="1"/>
+      <c r="J44" s="21"/>
       <c r="K44" s="20"/>
-      <c r="L44" s="1"/>
+      <c r="L44" s="21"/>
       <c r="M44" s="20"/>
+      <c r="N44" s="21"/>
       <c r="O44" s="20"/>
-    </row>
-    <row r="45" spans="1:15">
+      <c r="Q44" s="20"/>
+      <c r="R44" s="21"/>
+      <c r="S44" s="20"/>
+      <c r="T44" s="21"/>
+      <c r="U44" s="20"/>
+      <c r="V44" s="21"/>
+      <c r="W44" s="20"/>
+      <c r="X44" s="21"/>
+      <c r="Y44" s="20"/>
+      <c r="Z44" s="21"/>
+    </row>
+    <row r="45" spans="1:26">
       <c r="A45" s="20"/>
       <c r="B45" s="21"/>
       <c r="C45" s="20"/>
@@ -1391,14 +1644,26 @@
       <c r="E45" s="20"/>
       <c r="F45" s="21"/>
       <c r="G45" s="20"/>
+      <c r="H45" s="1"/>
       <c r="I45" s="20"/>
-      <c r="J45" s="1"/>
+      <c r="J45" s="21"/>
       <c r="K45" s="20"/>
-      <c r="L45" s="1"/>
+      <c r="L45" s="21"/>
       <c r="M45" s="20"/>
+      <c r="N45" s="21"/>
       <c r="O45" s="20"/>
-    </row>
-    <row r="46" spans="1:15">
+      <c r="Q45" s="20"/>
+      <c r="R45" s="21"/>
+      <c r="S45" s="20"/>
+      <c r="T45" s="21"/>
+      <c r="U45" s="20"/>
+      <c r="V45" s="21"/>
+      <c r="W45" s="20"/>
+      <c r="X45" s="21"/>
+      <c r="Y45" s="20"/>
+      <c r="Z45" s="21"/>
+    </row>
+    <row r="46" spans="1:26">
       <c r="A46" s="18"/>
       <c r="B46" s="18"/>
       <c r="C46" s="18"/>
@@ -1406,13 +1671,13 @@
       <c r="I46" s="1"/>
       <c r="J46" s="1"/>
     </row>
-    <row r="47" spans="1:15">
+    <row r="47" spans="1:26">
       <c r="E47" s="2" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="F47" s="1"/>
       <c r="G47" s="1"/>
-      <c r="H47" s="34">
+      <c r="H47" s="33">
         <f>SUM(H28+H31-H39)</f>
         <v>0</v>
       </c>
@@ -1421,13 +1686,13 @@
       <c r="K47" s="1"/>
       <c r="L47" s="1"/>
     </row>
-    <row r="48" spans="1:15">
+    <row r="48" spans="1:26">
       <c r="E48" s="2" t="s">
         <v>13</v>
       </c>
       <c r="F48" s="1"/>
       <c r="G48" s="1"/>
-      <c r="H48" s="35">
+      <c r="H48" s="34">
         <f>+H47-H25</f>
         <v>0</v>
       </c>

</xml_diff>